<commit_message>
Added functions of feeding animals and sending applications for the role of 'worker'
</commit_message>
<xml_diff>
--- a/Права Пользователей.xlsx
+++ b/Права Пользователей.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>Рабочий</t>
   </si>
@@ -78,9 +78,6 @@
     <t>animal_info</t>
   </si>
   <si>
-    <t>check_animal</t>
-  </si>
-  <si>
     <t>employee_info</t>
   </si>
   <si>
@@ -153,22 +150,25 @@
     <t>EXECUTE - исполнение</t>
   </si>
   <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>get_weighing_history</t>
+  </si>
+  <si>
+    <t>all_app_inspection</t>
+  </si>
+  <si>
+    <t>inspect</t>
+  </si>
+  <si>
     <t>SD</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>SU</t>
-  </si>
-  <si>
-    <t>get_weighing_history</t>
-  </si>
-  <si>
-    <t>all_app_inspection</t>
-  </si>
-  <si>
-    <t>inspect</t>
+    <t>all_app_change_feed</t>
+  </si>
+  <si>
+    <t>change_feed</t>
   </si>
 </sst>
 </file>
@@ -321,7 +321,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -351,27 +351,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -672,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
@@ -689,41 +684,41 @@
   <sheetData>
     <row r="1" spans="1:11" ht="57" customHeight="1">
       <c r="A1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="F1" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
+      <c r="G2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
     </row>
     <row r="3" spans="1:11" ht="37.5" customHeight="1">
       <c r="A3" s="5"/>
@@ -740,7 +735,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
@@ -762,18 +757,18 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="G4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1">
       <c r="A5" s="5" t="s">
@@ -781,18 +776,18 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="G5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1">
       <c r="A6" s="5" t="s">
@@ -803,15 +798,15 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="G6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
     </row>
     <row r="7" spans="1:11" ht="30" customHeight="1">
       <c r="A7" s="5" t="s">
@@ -819,20 +814,20 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="G7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:11" ht="30" customHeight="1">
       <c r="A8" s="5" t="s">
@@ -840,18 +835,20 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="G8" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:11" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
@@ -862,15 +859,17 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1">
       <c r="A10" s="5" t="s">
@@ -878,18 +877,18 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="G10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
@@ -900,13 +899,13 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="G11" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1">
       <c r="A12" s="5" t="s">
@@ -917,15 +916,15 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
+      <c r="G12" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
     </row>
     <row r="13" spans="1:11" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
@@ -933,31 +932,33 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
     </row>
     <row r="14" spans="1:11" ht="30" customHeight="1">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
     </row>
     <row r="15" spans="1:11" ht="37.5" customHeight="1">
       <c r="A15" s="7"/>
@@ -973,12 +974,14 @@
       <c r="E15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
+      <c r="F15" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
     </row>
     <row r="16" spans="1:11" ht="30" customHeight="1">
       <c r="A16" s="7" t="s">
@@ -986,12 +989,12 @@
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="12"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1005,8 +1008,8 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="12"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="11"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1018,12 +1021,12 @@
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="12"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1037,52 +1040,41 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
+      <c r="F19" s="15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="30" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="16"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:11" ht="30" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="16"/>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="1:11" ht="30" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="16"/>
+      <c r="F22" s="15"/>
     </row>
     <row r="23" spans="1:11" ht="30" customHeight="1">
       <c r="A23" s="7" t="s">
@@ -1092,7 +1084,7 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="16"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="1:11" ht="30" customHeight="1">
       <c r="A24" s="7" t="s">
@@ -1102,97 +1094,97 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="16"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="16"/>
+        <v>44</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="1:11" ht="30" customHeight="1">
-      <c r="A26" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="17"/>
+      <c r="A26" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="15"/>
       <c r="C26" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="16"/>
+        <v>41</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="1:11" ht="30" customHeight="1">
       <c r="A27" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="11"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="14"/>
+        <v>41</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
     </row>
     <row r="28" spans="1:11" ht="30" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="14"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
     </row>
     <row r="29" spans="1:11" ht="30" customHeight="1">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="8"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
     </row>
     <row r="30" spans="1:11" ht="30" customHeight="1">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="8"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
     </row>
     <row r="31" spans="1:11" ht="30" customHeight="1">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="8"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
     </row>
     <row r="32" spans="1:11" ht="30" customHeight="1">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="8"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
     </row>
     <row r="33" spans="1:6" ht="30" customHeight="1">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="8"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
     </row>
     <row r="34" spans="1:6" ht="30" customHeight="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="8"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:6" ht="30" customHeight="1">
       <c r="A35" s="2"/>
@@ -1297,14 +1289,6 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="8"/>
-    </row>
-    <row r="48" spans="1:6" ht="30" customHeight="1">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>